<commit_message>
updated the CreateResultsDF in main.py. change is made to prevent a mismatch that may occur.
</commit_message>
<xml_diff>
--- a/sap-results.xlsx
+++ b/sap-results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="84">
   <si>
     <t>MaintPlant</t>
   </si>
@@ -623,7 +623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC11"/>
+  <dimension ref="A1:AC21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -749,63 +749,6 @@
       <c r="J2" t="s">
         <v>66</v>
       </c>
-      <c r="K2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L2" t="s">
-        <v>67</v>
-      </c>
-      <c r="M2" t="s">
-        <v>67</v>
-      </c>
-      <c r="N2" t="s">
-        <v>67</v>
-      </c>
-      <c r="O2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T2" t="s">
-        <v>67</v>
-      </c>
-      <c r="U2" t="s">
-        <v>67</v>
-      </c>
-      <c r="V2" t="s">
-        <v>67</v>
-      </c>
-      <c r="W2" t="s">
-        <v>67</v>
-      </c>
-      <c r="X2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="3" spans="1:29">
       <c r="A3">
@@ -838,63 +781,6 @@
       <c r="J3" t="s">
         <v>66</v>
       </c>
-      <c r="K3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L3" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" t="s">
-        <v>67</v>
-      </c>
-      <c r="N3" t="s">
-        <v>67</v>
-      </c>
-      <c r="O3" t="s">
-        <v>67</v>
-      </c>
-      <c r="P3" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>67</v>
-      </c>
-      <c r="R3" t="s">
-        <v>67</v>
-      </c>
-      <c r="S3" t="s">
-        <v>67</v>
-      </c>
-      <c r="T3" t="s">
-        <v>67</v>
-      </c>
-      <c r="U3" t="s">
-        <v>67</v>
-      </c>
-      <c r="V3" t="s">
-        <v>67</v>
-      </c>
-      <c r="W3" t="s">
-        <v>67</v>
-      </c>
-      <c r="X3" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4">
@@ -927,63 +813,6 @@
       <c r="J4" t="s">
         <v>66</v>
       </c>
-      <c r="K4" t="s">
-        <v>67</v>
-      </c>
-      <c r="L4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M4" t="s">
-        <v>67</v>
-      </c>
-      <c r="N4" t="s">
-        <v>67</v>
-      </c>
-      <c r="O4" t="s">
-        <v>67</v>
-      </c>
-      <c r="P4" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>67</v>
-      </c>
-      <c r="R4" t="s">
-        <v>67</v>
-      </c>
-      <c r="S4" t="s">
-        <v>67</v>
-      </c>
-      <c r="T4" t="s">
-        <v>67</v>
-      </c>
-      <c r="U4" t="s">
-        <v>67</v>
-      </c>
-      <c r="V4" t="s">
-        <v>67</v>
-      </c>
-      <c r="W4" t="s">
-        <v>67</v>
-      </c>
-      <c r="X4" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5">
@@ -1016,63 +845,6 @@
       <c r="J5" t="s">
         <v>66</v>
       </c>
-      <c r="K5" t="s">
-        <v>67</v>
-      </c>
-      <c r="L5" t="s">
-        <v>67</v>
-      </c>
-      <c r="M5" t="s">
-        <v>67</v>
-      </c>
-      <c r="N5" t="s">
-        <v>67</v>
-      </c>
-      <c r="O5" t="s">
-        <v>67</v>
-      </c>
-      <c r="P5" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>67</v>
-      </c>
-      <c r="R5" t="s">
-        <v>67</v>
-      </c>
-      <c r="S5" t="s">
-        <v>67</v>
-      </c>
-      <c r="T5" t="s">
-        <v>67</v>
-      </c>
-      <c r="U5" t="s">
-        <v>67</v>
-      </c>
-      <c r="V5" t="s">
-        <v>67</v>
-      </c>
-      <c r="W5" t="s">
-        <v>67</v>
-      </c>
-      <c r="X5" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6">
@@ -1105,63 +877,6 @@
       <c r="J6" t="s">
         <v>66</v>
       </c>
-      <c r="K6" t="s">
-        <v>67</v>
-      </c>
-      <c r="L6" t="s">
-        <v>67</v>
-      </c>
-      <c r="M6" t="s">
-        <v>67</v>
-      </c>
-      <c r="N6" t="s">
-        <v>67</v>
-      </c>
-      <c r="O6" t="s">
-        <v>67</v>
-      </c>
-      <c r="P6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>67</v>
-      </c>
-      <c r="R6" t="s">
-        <v>67</v>
-      </c>
-      <c r="S6" t="s">
-        <v>67</v>
-      </c>
-      <c r="T6" t="s">
-        <v>67</v>
-      </c>
-      <c r="U6" t="s">
-        <v>67</v>
-      </c>
-      <c r="V6" t="s">
-        <v>67</v>
-      </c>
-      <c r="W6" t="s">
-        <v>67</v>
-      </c>
-      <c r="X6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="7" spans="1:29">
       <c r="A7">
@@ -1486,6 +1201,596 @@
       </c>
       <c r="AC11" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
+      <c r="K12" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" t="s">
+        <v>67</v>
+      </c>
+      <c r="M12" t="s">
+        <v>67</v>
+      </c>
+      <c r="N12" t="s">
+        <v>67</v>
+      </c>
+      <c r="O12" t="s">
+        <v>67</v>
+      </c>
+      <c r="P12" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>67</v>
+      </c>
+      <c r="R12" t="s">
+        <v>67</v>
+      </c>
+      <c r="S12" t="s">
+        <v>67</v>
+      </c>
+      <c r="T12" t="s">
+        <v>67</v>
+      </c>
+      <c r="U12" t="s">
+        <v>67</v>
+      </c>
+      <c r="V12" t="s">
+        <v>67</v>
+      </c>
+      <c r="W12" t="s">
+        <v>67</v>
+      </c>
+      <c r="X12" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
+      <c r="K13" t="s">
+        <v>67</v>
+      </c>
+      <c r="L13" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13" t="s">
+        <v>67</v>
+      </c>
+      <c r="N13" t="s">
+        <v>67</v>
+      </c>
+      <c r="O13" t="s">
+        <v>67</v>
+      </c>
+      <c r="P13" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>67</v>
+      </c>
+      <c r="R13" t="s">
+        <v>67</v>
+      </c>
+      <c r="S13" t="s">
+        <v>67</v>
+      </c>
+      <c r="T13" t="s">
+        <v>67</v>
+      </c>
+      <c r="U13" t="s">
+        <v>67</v>
+      </c>
+      <c r="V13" t="s">
+        <v>67</v>
+      </c>
+      <c r="W13" t="s">
+        <v>67</v>
+      </c>
+      <c r="X13" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
+      <c r="K14" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14" t="s">
+        <v>67</v>
+      </c>
+      <c r="N14" t="s">
+        <v>67</v>
+      </c>
+      <c r="O14" t="s">
+        <v>67</v>
+      </c>
+      <c r="P14" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>67</v>
+      </c>
+      <c r="R14" t="s">
+        <v>67</v>
+      </c>
+      <c r="S14" t="s">
+        <v>67</v>
+      </c>
+      <c r="T14" t="s">
+        <v>67</v>
+      </c>
+      <c r="U14" t="s">
+        <v>67</v>
+      </c>
+      <c r="V14" t="s">
+        <v>67</v>
+      </c>
+      <c r="W14" t="s">
+        <v>67</v>
+      </c>
+      <c r="X14" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
+      <c r="K15" t="s">
+        <v>67</v>
+      </c>
+      <c r="L15" t="s">
+        <v>67</v>
+      </c>
+      <c r="M15" t="s">
+        <v>67</v>
+      </c>
+      <c r="N15" t="s">
+        <v>67</v>
+      </c>
+      <c r="O15" t="s">
+        <v>67</v>
+      </c>
+      <c r="P15" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>67</v>
+      </c>
+      <c r="R15" t="s">
+        <v>67</v>
+      </c>
+      <c r="S15" t="s">
+        <v>67</v>
+      </c>
+      <c r="T15" t="s">
+        <v>67</v>
+      </c>
+      <c r="U15" t="s">
+        <v>67</v>
+      </c>
+      <c r="V15" t="s">
+        <v>67</v>
+      </c>
+      <c r="W15" t="s">
+        <v>67</v>
+      </c>
+      <c r="X15" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
+      <c r="K16" t="s">
+        <v>67</v>
+      </c>
+      <c r="L16" t="s">
+        <v>67</v>
+      </c>
+      <c r="M16" t="s">
+        <v>67</v>
+      </c>
+      <c r="N16" t="s">
+        <v>67</v>
+      </c>
+      <c r="O16" t="s">
+        <v>67</v>
+      </c>
+      <c r="P16" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>67</v>
+      </c>
+      <c r="R16" t="s">
+        <v>67</v>
+      </c>
+      <c r="S16" t="s">
+        <v>67</v>
+      </c>
+      <c r="T16" t="s">
+        <v>67</v>
+      </c>
+      <c r="U16" t="s">
+        <v>67</v>
+      </c>
+      <c r="V16" t="s">
+        <v>67</v>
+      </c>
+      <c r="W16" t="s">
+        <v>67</v>
+      </c>
+      <c r="X16" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="11:29">
+      <c r="K17" t="s">
+        <v>67</v>
+      </c>
+      <c r="L17" t="s">
+        <v>67</v>
+      </c>
+      <c r="M17" t="s">
+        <v>67</v>
+      </c>
+      <c r="N17" t="s">
+        <v>67</v>
+      </c>
+      <c r="O17" t="s">
+        <v>67</v>
+      </c>
+      <c r="P17" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>67</v>
+      </c>
+      <c r="R17" t="s">
+        <v>67</v>
+      </c>
+      <c r="S17" t="s">
+        <v>67</v>
+      </c>
+      <c r="T17" t="s">
+        <v>67</v>
+      </c>
+      <c r="U17" t="s">
+        <v>67</v>
+      </c>
+      <c r="V17" t="s">
+        <v>67</v>
+      </c>
+      <c r="W17" t="s">
+        <v>67</v>
+      </c>
+      <c r="X17" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="11:29">
+      <c r="K18" t="s">
+        <v>67</v>
+      </c>
+      <c r="L18" t="s">
+        <v>67</v>
+      </c>
+      <c r="M18" t="s">
+        <v>67</v>
+      </c>
+      <c r="N18" t="s">
+        <v>67</v>
+      </c>
+      <c r="O18" t="s">
+        <v>67</v>
+      </c>
+      <c r="P18" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>67</v>
+      </c>
+      <c r="R18" t="s">
+        <v>67</v>
+      </c>
+      <c r="S18" t="s">
+        <v>67</v>
+      </c>
+      <c r="T18" t="s">
+        <v>67</v>
+      </c>
+      <c r="U18" t="s">
+        <v>67</v>
+      </c>
+      <c r="V18" t="s">
+        <v>67</v>
+      </c>
+      <c r="W18" t="s">
+        <v>67</v>
+      </c>
+      <c r="X18" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="11:29">
+      <c r="K19" t="s">
+        <v>67</v>
+      </c>
+      <c r="L19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M19" t="s">
+        <v>67</v>
+      </c>
+      <c r="N19" t="s">
+        <v>67</v>
+      </c>
+      <c r="O19" t="s">
+        <v>67</v>
+      </c>
+      <c r="P19" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>67</v>
+      </c>
+      <c r="R19" t="s">
+        <v>67</v>
+      </c>
+      <c r="S19" t="s">
+        <v>67</v>
+      </c>
+      <c r="T19" t="s">
+        <v>67</v>
+      </c>
+      <c r="U19" t="s">
+        <v>67</v>
+      </c>
+      <c r="V19" t="s">
+        <v>67</v>
+      </c>
+      <c r="W19" t="s">
+        <v>67</v>
+      </c>
+      <c r="X19" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="11:29">
+      <c r="K20" t="s">
+        <v>67</v>
+      </c>
+      <c r="L20" t="s">
+        <v>67</v>
+      </c>
+      <c r="M20" t="s">
+        <v>67</v>
+      </c>
+      <c r="N20" t="s">
+        <v>67</v>
+      </c>
+      <c r="O20" t="s">
+        <v>67</v>
+      </c>
+      <c r="P20" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>67</v>
+      </c>
+      <c r="R20" t="s">
+        <v>67</v>
+      </c>
+      <c r="S20" t="s">
+        <v>67</v>
+      </c>
+      <c r="T20" t="s">
+        <v>67</v>
+      </c>
+      <c r="U20" t="s">
+        <v>67</v>
+      </c>
+      <c r="V20" t="s">
+        <v>67</v>
+      </c>
+      <c r="W20" t="s">
+        <v>67</v>
+      </c>
+      <c r="X20" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="11:29">
+      <c r="K21" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21" t="s">
+        <v>67</v>
+      </c>
+      <c r="M21" t="s">
+        <v>67</v>
+      </c>
+      <c r="N21" t="s">
+        <v>67</v>
+      </c>
+      <c r="O21" t="s">
+        <v>67</v>
+      </c>
+      <c r="P21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>67</v>
+      </c>
+      <c r="R21" t="s">
+        <v>67</v>
+      </c>
+      <c r="S21" t="s">
+        <v>67</v>
+      </c>
+      <c r="T21" t="s">
+        <v>67</v>
+      </c>
+      <c r="U21" t="s">
+        <v>67</v>
+      </c>
+      <c r="V21" t="s">
+        <v>67</v>
+      </c>
+      <c r="W21" t="s">
+        <v>67</v>
+      </c>
+      <c r="X21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>